<commit_message>
starting line charts. restarted from scratch using the DOM provided
</commit_message>
<xml_diff>
--- a/HW2/hT5la9Cq2b_hw2/HW2/Q1/Q1-1.xlsx
+++ b/HW2/hT5la9Cq2b_hw2/HW2/Q1/Q1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c14cc3b5b526ad28/OMSA/Fall 2024/Homework/CS6242/HW2/hT5la9Cq2b_hw2/HW2/Q1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{23C29C92-E197-4865-A147-131E803897DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7C65D1-A74E-46B7-BE27-EA29FC01B803}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{23C29C92-E197-4865-A147-131E803897DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48E8FC4B-F1A4-4613-BCEF-400880E642B6}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{4DCEF8E0-F32B-46A7-8C15-8A2877788DB8}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>Avg. Rating</t>
   </si>
   <si>
-    <t>Sherlock Holmes Consulting Detective...</t>
-  </si>
-  <si>
     <t>No. Games</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>Popular Board Games</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes Consulting Detective: The Thames Murders &amp; Other Cases</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P25" sqref="N25:P26"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -678,13 +678,13 @@
     <col min="1" max="1" width="21.3046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.15234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.3828125" customWidth="1"/>
-    <col min="4" max="4" width="35.4609375" customWidth="1"/>
+    <col min="4" max="4" width="36.921875" customWidth="1"/>
     <col min="5" max="6" width="12.921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -698,7 +698,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>44</v>
@@ -710,7 +710,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -721,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -748,7 +748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -766,7 +766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -785,7 +785,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -805,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -859,7 +859,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -889,6 +889,6 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="81" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>